<commit_message>
testandomedidad de disperão despad no emsemble metrics
</commit_message>
<xml_diff>
--- a/fuction_ensemble_1/redes-ensemble-s/Teste03/content/results/metrics_10_2.xlsx
+++ b/fuction_ensemble_1/redes-ensemble-s/Teste03/content/results/metrics_10_2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,771 +518,771 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_0</t>
+          <t>model_10_2_8</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9997902228775151</v>
+        <v>0.3011264900069626</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6313074241689618</v>
+        <v>-0.4291036708362139</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9997468045287514</v>
+        <v>-0.4721940443070574</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9998859555735164</v>
+        <v>-29.40584381553866</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9998457739684059</v>
+        <v>-1.734333692991516</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0001245327618069041</v>
+        <v>0.4148815052955427</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2188718397032906</v>
+        <v>0.848377673072515</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0001480262243843989</v>
+        <v>0.5377293661538703</v>
       </c>
       <c r="J2" t="n">
-        <v>3.899569344622645e-05</v>
+        <v>0.9086532672472513</v>
       </c>
       <c r="K2" t="n">
-        <v>9.351095891531268e-05</v>
+        <v>0.7231913167005608</v>
       </c>
       <c r="L2" t="n">
-        <v>0.005210080280164223</v>
+        <v>0.2650272797837775</v>
       </c>
       <c r="M2" t="n">
-        <v>0.01115942479731389</v>
+        <v>0.6441129600431454</v>
       </c>
       <c r="N2" t="n">
-        <v>1.000111881131992</v>
+        <v>-1.096620529979112</v>
       </c>
       <c r="O2" t="n">
-        <v>0.01163450461412948</v>
+        <v>0.6715341822498224</v>
       </c>
       <c r="P2" t="n">
-        <v>155.9818834592664</v>
+        <v>33.7595246578621</v>
       </c>
       <c r="Q2" t="n">
-        <v>240.0843153751723</v>
+        <v>53.26153785575331</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_1</t>
+          <t>model_10_2_11</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9998334263569202</v>
+        <v>0.2762754434122477</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6311227469266392</v>
+        <v>-0.6364057929662033</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9998043947601526</v>
+        <v>-0.6332599521602595</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9999250111660326</v>
+        <v>-32.81133008180126</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9998845515363393</v>
+        <v>-2.037943251359588</v>
       </c>
       <c r="G3" t="n">
-        <v>9.888531013890318e-05</v>
+        <v>0.4296341600634815</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2189814720919747</v>
+        <v>0.971441167754274</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0001143571209296657</v>
+        <v>0.5965598368203009</v>
       </c>
       <c r="J3" t="n">
-        <v>2.564124939244895e-05</v>
+        <v>1.010423382267831</v>
       </c>
       <c r="K3" t="n">
-        <v>6.999918516105734e-05</v>
+        <v>0.803491609544066</v>
       </c>
       <c r="L3" t="n">
-        <v>0.004598027716036268</v>
+        <v>0.2540161354991849</v>
       </c>
       <c r="M3" t="n">
-        <v>0.009944109318531407</v>
+        <v>0.6554648427364214</v>
       </c>
       <c r="N3" t="n">
-        <v>1.000088839276309</v>
+        <v>-1.171173669763257</v>
       </c>
       <c r="O3" t="n">
-        <v>0.01036745063936537</v>
+        <v>0.6833693380909878</v>
       </c>
       <c r="P3" t="n">
-        <v>156.4430997256715</v>
+        <v>33.68964244594453</v>
       </c>
       <c r="Q3" t="n">
-        <v>240.5455316415774</v>
+        <v>53.19165564383574</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_2</t>
+          <t>model_10_2_10</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9998671370124151</v>
+        <v>0.2811272057860386</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6309353383765102</v>
+        <v>-0.6521431390776447</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9998462664630586</v>
+        <v>-0.6061389946012343</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9999512193091653</v>
+        <v>-32.41121149527143</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9999121280603382</v>
+        <v>-1.996611416438533</v>
       </c>
       <c r="G4" t="n">
-        <v>7.887320881256716e-05</v>
+        <v>0.4267539443331777</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2190927259029592</v>
+        <v>0.9807835362239801</v>
       </c>
       <c r="I4" t="n">
-        <v>8.987757530763684e-05</v>
+        <v>0.5866537137965762</v>
       </c>
       <c r="J4" t="n">
-        <v>1.667978808380514e-05</v>
+        <v>0.9984661722281321</v>
       </c>
       <c r="K4" t="n">
-        <v>5.327887422498375e-05</v>
+        <v>0.7925599430123541</v>
       </c>
       <c r="L4" t="n">
-        <v>0.004116811266837755</v>
+        <v>0.2546110488123543</v>
       </c>
       <c r="M4" t="n">
-        <v>0.008881058991616212</v>
+        <v>0.6532640693725453</v>
       </c>
       <c r="N4" t="n">
-        <v>1.000070860260045</v>
+        <v>-1.156618382641884</v>
       </c>
       <c r="O4" t="n">
-        <v>0.009259144059215848</v>
+        <v>0.6810748732487827</v>
       </c>
       <c r="P4" t="n">
-        <v>156.8953378931033</v>
+        <v>33.70309534924927</v>
       </c>
       <c r="Q4" t="n">
-        <v>240.9977698090092</v>
+        <v>53.20510854714048</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_3</t>
+          <t>model_10_2_19</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9998931199388109</v>
+        <v>0.2223997940426102</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6307468279912624</v>
+        <v>-0.6615724668550349</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9998751389949726</v>
+        <v>-0.9018359647718295</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9999672063700935</v>
+        <v>-36.83123377798387</v>
       </c>
       <c r="F5" t="n">
-        <v>0.99993055600822</v>
+        <v>-2.450500573866818</v>
       </c>
       <c r="G5" t="n">
-        <v>6.344862130010173e-05</v>
+        <v>0.4616170728361702</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2192046338108669</v>
+        <v>0.9863811925183898</v>
       </c>
       <c r="I5" t="n">
-        <v>7.299776356941148e-05</v>
+        <v>0.6946591394117134</v>
       </c>
       <c r="J5" t="n">
-        <v>1.121326467461559e-05</v>
+        <v>1.130554849419845</v>
       </c>
       <c r="K5" t="n">
-        <v>4.210556541675986e-05</v>
+        <v>0.912606994415779</v>
       </c>
       <c r="L5" t="n">
-        <v>0.003678824211901579</v>
+        <v>0.2569582166269004</v>
       </c>
       <c r="M5" t="n">
-        <v>0.007965464286537334</v>
+        <v>0.6794240743719421</v>
       </c>
       <c r="N5" t="n">
-        <v>1.000057002699301</v>
+        <v>-1.332800617872169</v>
       </c>
       <c r="O5" t="n">
-        <v>0.008304570591999436</v>
+        <v>0.7083485638196794</v>
       </c>
       <c r="P5" t="n">
-        <v>157.3305601859175</v>
+        <v>33.54603915651736</v>
       </c>
       <c r="Q5" t="n">
-        <v>241.4329921018233</v>
+        <v>53.04805235440857</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_4</t>
+          <t>model_10_2_17</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9999128465282562</v>
+        <v>0.2238494182176843</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6305605096040694</v>
+        <v>-0.663962086842101</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9998933180442648</v>
+        <v>-0.8970955983210271</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9999749909664744</v>
+        <v>-36.70719747040197</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9999415154371633</v>
+        <v>-2.440219903658196</v>
       </c>
       <c r="G6" t="n">
-        <v>5.173806566109244e-05</v>
+        <v>0.4607565133053424</v>
       </c>
       <c r="H6" t="n">
-        <v>0.2193152404540399</v>
+        <v>0.9877997741689207</v>
       </c>
       <c r="I6" t="n">
-        <v>6.23697060597025e-05</v>
+        <v>0.6929276867837232</v>
       </c>
       <c r="J6" t="n">
-        <v>8.551444685417819e-06</v>
+        <v>1.126848127882191</v>
       </c>
       <c r="K6" t="n">
-        <v>3.546059958933141e-05</v>
+        <v>0.9098879073329572</v>
       </c>
       <c r="L6" t="n">
-        <v>0.00331692370952786</v>
+        <v>0.2568294898628027</v>
       </c>
       <c r="M6" t="n">
-        <v>0.007192917743245257</v>
+        <v>0.6787904782076295</v>
       </c>
       <c r="N6" t="n">
-        <v>1.000046481851597</v>
+        <v>-1.328451745346947</v>
       </c>
       <c r="O6" t="n">
-        <v>0.007499135142967607</v>
+        <v>0.7076879941549272</v>
       </c>
       <c r="P6" t="n">
-        <v>157.7386335353183</v>
+        <v>33.54977109244203</v>
       </c>
       <c r="Q6" t="n">
-        <v>241.8410654512242</v>
+        <v>53.05178429033324</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_5</t>
+          <t>model_10_2_23</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9999275045159596</v>
+        <v>0.2218058683462298</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6303779051047151</v>
+        <v>-0.6648634307852561</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9999027186286261</v>
+        <v>-0.9038315922941766</v>
       </c>
       <c r="E7" t="n">
-        <v>0.999976293824683</v>
+        <v>-36.8816104617073</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9999464149823</v>
+        <v>-2.454724592279671</v>
       </c>
       <c r="G7" t="n">
-        <v>4.303645096821314e-05</v>
+        <v>0.4619696527857958</v>
       </c>
       <c r="H7" t="n">
-        <v>0.2194236423729602</v>
+        <v>0.9883348508696086</v>
       </c>
       <c r="I7" t="n">
-        <v>5.687382178048259e-05</v>
+        <v>0.6953880565859274</v>
       </c>
       <c r="J7" t="n">
-        <v>8.105952863711868e-06</v>
+        <v>1.132060314571086</v>
       </c>
       <c r="K7" t="n">
-        <v>3.248988732209722e-05</v>
+        <v>0.9137241855785067</v>
       </c>
       <c r="L7" t="n">
-        <v>0.003035000303651324</v>
+        <v>0.2569852858699754</v>
       </c>
       <c r="M7" t="n">
-        <v>0.006560217295807597</v>
+        <v>0.6796834945662545</v>
       </c>
       <c r="N7" t="n">
-        <v>1.000038664258155</v>
+        <v>-1.33458239496131</v>
       </c>
       <c r="O7" t="n">
-        <v>0.006839499327612043</v>
+        <v>0.7086190280687377</v>
       </c>
       <c r="P7" t="n">
-        <v>158.1069262088553</v>
+        <v>33.54451215333738</v>
       </c>
       <c r="Q7" t="n">
-        <v>242.2093581247611</v>
+        <v>53.04652535122859</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_6</t>
+          <t>model_10_2_21</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.999938076554415</v>
+        <v>0.2218058406824498</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6302006465317724</v>
+        <v>-0.6648635541388184</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9999049954976303</v>
+        <v>-0.9038315922941766</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9999725186717043</v>
+        <v>-36.8816104617073</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9999464484671495</v>
+        <v>-2.454724592279671</v>
       </c>
       <c r="G8" t="n">
-        <v>3.676043225282087e-05</v>
+        <v>0.4619696692082106</v>
       </c>
       <c r="H8" t="n">
-        <v>0.2195288707190307</v>
+        <v>0.9883349240976118</v>
       </c>
       <c r="I8" t="n">
-        <v>5.554269085445157e-05</v>
+        <v>0.6953880565859274</v>
       </c>
       <c r="J8" t="n">
-        <v>9.396806900228003e-06</v>
+        <v>1.132060314571086</v>
       </c>
       <c r="K8" t="n">
-        <v>3.246958465100894e-05</v>
+        <v>0.9137241855785067</v>
       </c>
       <c r="L8" t="n">
-        <v>0.002779213374212671</v>
+        <v>0.2569860898984025</v>
       </c>
       <c r="M8" t="n">
-        <v>0.006063038203147072</v>
+        <v>0.6796835066471826</v>
       </c>
       <c r="N8" t="n">
-        <v>1.000033025837645</v>
+        <v>-1.334582477952651</v>
       </c>
       <c r="O8" t="n">
-        <v>0.006321154291674356</v>
+        <v>0.7086190406639757</v>
       </c>
       <c r="P8" t="n">
-        <v>158.4221770035281</v>
+        <v>33.54451208224</v>
       </c>
       <c r="Q8" t="n">
-        <v>242.524608919434</v>
+        <v>53.04652528013121</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_7</t>
+          <t>model_10_2_20</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9999453221161051</v>
+        <v>0.2218055075618536</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6300309389258434</v>
+        <v>-0.6648636017286398</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9999013762288842</v>
+        <v>-0.9038349761223379</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9999646783518733</v>
+        <v>-36.8816104617073</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9999424925438425</v>
+        <v>-2.454726928830934</v>
       </c>
       <c r="G9" t="n">
-        <v>3.245915384159691e-05</v>
+        <v>0.4619698669629866</v>
       </c>
       <c r="H9" t="n">
-        <v>0.219629616484897</v>
+        <v>0.9883349523489855</v>
       </c>
       <c r="I9" t="n">
-        <v>5.765863188953408e-05</v>
+        <v>0.6953892925532779</v>
       </c>
       <c r="J9" t="n">
-        <v>1.207768064458973e-05</v>
+        <v>1.132060314571086</v>
       </c>
       <c r="K9" t="n">
-        <v>3.48681562670619e-05</v>
+        <v>0.9137248035621818</v>
       </c>
       <c r="L9" t="n">
-        <v>0.002548133726527339</v>
+        <v>0.2569861633915473</v>
       </c>
       <c r="M9" t="n">
-        <v>0.005697293554100658</v>
+        <v>0.6796836521227994</v>
       </c>
       <c r="N9" t="n">
-        <v>1.000029161538077</v>
+        <v>-1.334583477314439</v>
       </c>
       <c r="O9" t="n">
-        <v>0.005939839135722238</v>
+        <v>0.7086191923327908</v>
       </c>
       <c r="P9" t="n">
-        <v>158.6710561278882</v>
+        <v>33.5445112261027</v>
       </c>
       <c r="Q9" t="n">
-        <v>242.7734880437941</v>
+        <v>53.04652442399391</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_8</t>
+          <t>model_10_2_22</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9999498616506092</v>
+        <v>0.2218055075618536</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6298704552496563</v>
+        <v>-0.6648638145372905</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9998928852208169</v>
+        <v>-0.9038349761223379</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9999535323931268</v>
+        <v>-36.8816104617073</v>
       </c>
       <c r="F10" t="n">
-        <v>0.999935256066168</v>
+        <v>-2.454726928830934</v>
       </c>
       <c r="G10" t="n">
-        <v>2.976429006231161e-05</v>
+        <v>0.4619698669629866</v>
       </c>
       <c r="H10" t="n">
-        <v>0.2197248865276155</v>
+        <v>0.9883350786813935</v>
       </c>
       <c r="I10" t="n">
-        <v>6.262274858255744e-05</v>
+        <v>0.6953892925532779</v>
       </c>
       <c r="J10" t="n">
-        <v>1.588886549461948e-05</v>
+        <v>1.132060314571086</v>
       </c>
       <c r="K10" t="n">
-        <v>3.925580703858847e-05</v>
+        <v>0.9137248035621818</v>
       </c>
       <c r="L10" t="n">
-        <v>0.002339839765250848</v>
+        <v>0.2569861633915473</v>
       </c>
       <c r="M10" t="n">
-        <v>0.005455665867913065</v>
+        <v>0.6796836521227994</v>
       </c>
       <c r="N10" t="n">
-        <v>1.000026740453009</v>
+        <v>-1.334583477314439</v>
       </c>
       <c r="O10" t="n">
-        <v>0.005687924858695374</v>
+        <v>0.7086191923327908</v>
       </c>
       <c r="P10" t="n">
-        <v>158.8444024061383</v>
+        <v>33.5445112261027</v>
       </c>
       <c r="Q10" t="n">
-        <v>242.9468343220441</v>
+        <v>53.04652442399391</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_9</t>
+          <t>model_10_2_18</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.9999522414398366</v>
+        <v>0.2225819472702458</v>
       </c>
       <c r="C11" t="n">
-        <v>0.6297201948183304</v>
+        <v>-0.6678499268264624</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9998805460626007</v>
+        <v>-0.901990067378708</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9999398829891722</v>
+        <v>-36.80661520843953</v>
       </c>
       <c r="F11" t="n">
-        <v>0.999925458444942</v>
+        <v>-2.449216158257414</v>
       </c>
       <c r="G11" t="n">
-        <v>2.835154437533546e-05</v>
+        <v>0.461508938811636</v>
       </c>
       <c r="H11" t="n">
-        <v>0.2198140876105633</v>
+        <v>0.9901077639295802</v>
       </c>
       <c r="I11" t="n">
-        <v>6.983661774782333e-05</v>
+        <v>0.6947154264870755</v>
       </c>
       <c r="J11" t="n">
-        <v>2.055606396057193e-05</v>
+        <v>1.129819144014425</v>
       </c>
       <c r="K11" t="n">
-        <v>4.519634085419763e-05</v>
+        <v>0.9122672852507504</v>
       </c>
       <c r="L11" t="n">
-        <v>0.002152101353041621</v>
+        <v>0.2568991522493798</v>
       </c>
       <c r="M11" t="n">
-        <v>0.005324616828968584</v>
+        <v>0.6793444920006608</v>
       </c>
       <c r="N11" t="n">
-        <v>1.000025471232087</v>
+        <v>-1.332254158189262</v>
       </c>
       <c r="O11" t="n">
-        <v>0.005551296790854119</v>
+        <v>0.7082655934620946</v>
       </c>
       <c r="P11" t="n">
-        <v>158.9416581079075</v>
+        <v>33.54650771237502</v>
       </c>
       <c r="Q11" t="n">
-        <v>243.0440900238134</v>
+        <v>53.04852091026623</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_10</t>
+          <t>model_10_2_16</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.9999528475304226</v>
+        <v>0.2264660371641365</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6295760381315174</v>
+        <v>-0.6729179866784996</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9998649564972877</v>
+        <v>-0.8881248410507727</v>
       </c>
       <c r="E12" t="n">
-        <v>0.99992416811804</v>
+        <v>-36.48857218820502</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9999135113960407</v>
+        <v>-2.421674329024688</v>
       </c>
       <c r="G12" t="n">
-        <v>2.799174282179029e-05</v>
+        <v>0.4592031752666754</v>
       </c>
       <c r="H12" t="n">
-        <v>0.2198996652471001</v>
+        <v>0.9931163831865356</v>
       </c>
       <c r="I12" t="n">
-        <v>7.895077955216381e-05</v>
+        <v>0.6896510537613931</v>
       </c>
       <c r="J12" t="n">
-        <v>2.59295163608098e-05</v>
+        <v>1.120314693777344</v>
       </c>
       <c r="K12" t="n">
-        <v>5.244012445817231e-05</v>
+        <v>0.9049828737693685</v>
       </c>
       <c r="L12" t="n">
-        <v>0.001982801775650941</v>
+        <v>0.2565556132308984</v>
       </c>
       <c r="M12" t="n">
-        <v>0.005290722334595749</v>
+        <v>0.6776453167156661</v>
       </c>
       <c r="N12" t="n">
-        <v>1.000025147983775</v>
+        <v>-1.320601888507591</v>
       </c>
       <c r="O12" t="n">
-        <v>0.005515959337684556</v>
+        <v>0.7064940807674398</v>
       </c>
       <c r="P12" t="n">
-        <v>158.9672019810043</v>
+        <v>33.55652503844269</v>
       </c>
       <c r="Q12" t="n">
-        <v>243.0696338969102</v>
+        <v>53.0585382363339</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_11</t>
+          <t>model_10_2_13</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9999519805406603</v>
+        <v>0.2469434911351397</v>
       </c>
       <c r="C13" t="n">
-        <v>0.6294424552466789</v>
+        <v>-0.673966572728999</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9998465771810061</v>
+        <v>-0.800126016462064</v>
       </c>
       <c r="E13" t="n">
-        <v>0.9999065876218972</v>
+        <v>-34.91671150388402</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9998996932411532</v>
+        <v>-2.272108520932408</v>
       </c>
       <c r="G13" t="n">
-        <v>2.850642539668895e-05</v>
+        <v>0.4470468740095357</v>
       </c>
       <c r="H13" t="n">
-        <v>0.2199789658180204</v>
+        <v>0.993738869162671</v>
       </c>
       <c r="I13" t="n">
-        <v>8.969591959159843e-05</v>
+        <v>0.6575088559639251</v>
       </c>
       <c r="J13" t="n">
-        <v>3.194088981723606e-05</v>
+        <v>1.073340949021874</v>
       </c>
       <c r="K13" t="n">
-        <v>6.081840470441724e-05</v>
+        <v>0.8654249024928995</v>
       </c>
       <c r="L13" t="n">
-        <v>0.001868472950868992</v>
+        <v>0.2547343181609897</v>
       </c>
       <c r="M13" t="n">
-        <v>0.005339140885637778</v>
+        <v>0.6686156399677887</v>
       </c>
       <c r="N13" t="n">
-        <v>1.000025610378315</v>
+        <v>-1.259169526594581</v>
       </c>
       <c r="O13" t="n">
-        <v>0.005566439166684662</v>
+        <v>0.6970799919863977</v>
       </c>
       <c r="P13" t="n">
-        <v>158.9307620871697</v>
+        <v>33.61018365262072</v>
       </c>
       <c r="Q13" t="n">
-        <v>243.0331940030756</v>
+        <v>53.11219685051193</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_12</t>
+          <t>model_10_2_15</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.9999498736225504</v>
+        <v>0.2321097179606092</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6293191367996436</v>
+        <v>-0.6766021094716062</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9998257807773526</v>
+        <v>-0.8663351661222305</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9998872849197322</v>
+        <v>-36.03586192828269</v>
       </c>
       <c r="F14" t="n">
-        <v>0.999884223598013</v>
+        <v>-2.381052610270964</v>
       </c>
       <c r="G14" t="n">
-        <v>2.975718300085267e-05</v>
+        <v>0.455852842551573</v>
       </c>
       <c r="H14" t="n">
-        <v>0.22005217297526</v>
+        <v>0.9953034376223417</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0001018541667293464</v>
+        <v>0.6816922197114029</v>
       </c>
       <c r="J14" t="n">
-        <v>3.854114446816504e-05</v>
+        <v>1.106785825468662</v>
       </c>
       <c r="K14" t="n">
-        <v>7.019802206975192e-05</v>
+        <v>0.8942390225900323</v>
       </c>
       <c r="L14" t="n">
-        <v>0.001787080627850092</v>
+        <v>0.2560369260868807</v>
       </c>
       <c r="M14" t="n">
-        <v>0.005455014482185421</v>
+        <v>0.6751687511663829</v>
       </c>
       <c r="N14" t="n">
-        <v>1.000026734067973</v>
+        <v>-1.303670846118172</v>
       </c>
       <c r="O14" t="n">
-        <v>0.00568724574212875</v>
+        <v>0.7039120826955262</v>
       </c>
       <c r="P14" t="n">
-        <v>158.8448800194182</v>
+        <v>33.57117047050743</v>
       </c>
       <c r="Q14" t="n">
-        <v>242.947311935324</v>
+        <v>53.07318366839863</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_13</t>
+          <t>model_10_2_12</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.999946675601582</v>
+        <v>0.2494262025755959</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6291983094531554</v>
+        <v>-0.6802067264899538</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9998026163940394</v>
+        <v>-0.7893680669204033</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9998663702913513</v>
+        <v>-34.71782946681531</v>
       </c>
       <c r="F15" t="n">
-        <v>0.999867158351996</v>
+        <v>-2.253444273753013</v>
       </c>
       <c r="G15" t="n">
-        <v>3.165566639498884e-05</v>
+        <v>0.445573029250931</v>
       </c>
       <c r="H15" t="n">
-        <v>0.2201239013076051</v>
+        <v>0.9974432939957804</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0001153968110157561</v>
+        <v>0.653579438228184</v>
       </c>
       <c r="J15" t="n">
-        <v>4.569257187266109e-05</v>
+        <v>1.06739752532097</v>
       </c>
       <c r="K15" t="n">
-        <v>8.054509190401658e-05</v>
+        <v>0.8604884817745768</v>
       </c>
       <c r="L15" t="n">
-        <v>0.001796168970146148</v>
+        <v>0.2545006090233257</v>
       </c>
       <c r="M15" t="n">
-        <v>0.005626336854027569</v>
+        <v>0.6675125686089596</v>
       </c>
       <c r="N15" t="n">
-        <v>1.000028439679156</v>
+        <v>-1.251721392273212</v>
       </c>
       <c r="O15" t="n">
-        <v>0.005865861662026419</v>
+        <v>0.6959299605961506</v>
       </c>
       <c r="P15" t="n">
-        <v>158.7211867847631</v>
+        <v>33.61678823803314</v>
       </c>
       <c r="Q15" t="n">
-        <v>242.823618700669</v>
+        <v>53.11880143592435</v>
       </c>
     </row>
     <row r="16">
@@ -1292,602 +1292,547 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.9999426532415755</v>
+        <v>0.2331459913687646</v>
       </c>
       <c r="C16" t="n">
-        <v>0.6290895074757439</v>
+        <v>-0.6850223783240319</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9997778534028081</v>
+        <v>-0.8627322137910156</v>
       </c>
       <c r="E16" t="n">
-        <v>0.999844237907731</v>
+        <v>-35.94782810385416</v>
       </c>
       <c r="F16" t="n">
-        <v>0.9998489797402259</v>
+        <v>-2.373591288172263</v>
       </c>
       <c r="G16" t="n">
-        <v>3.404351305173307e-05</v>
+        <v>0.4552376658918116</v>
       </c>
       <c r="H16" t="n">
-        <v>0.2201884908613972</v>
+        <v>1.000302072949817</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0001298740529599616</v>
+        <v>0.6803762156962809</v>
       </c>
       <c r="J16" t="n">
-        <v>5.326039148034063e-05</v>
+        <v>1.104155008094194</v>
       </c>
       <c r="K16" t="n">
-        <v>9.156722222015109e-05</v>
+        <v>0.8922656118952377</v>
       </c>
       <c r="L16" t="n">
-        <v>0.001824289149989091</v>
+        <v>0.2559020818519206</v>
       </c>
       <c r="M16" t="n">
-        <v>0.005834681915214665</v>
+        <v>0.6747130248422744</v>
       </c>
       <c r="N16" t="n">
-        <v>1.000030584937826</v>
+        <v>-1.300562025893706</v>
       </c>
       <c r="O16" t="n">
-        <v>0.006083076403801983</v>
+        <v>0.7034369551583168</v>
       </c>
       <c r="P16" t="n">
-        <v>158.5757421118986</v>
+        <v>33.57387130757048</v>
       </c>
       <c r="Q16" t="n">
-        <v>242.6781740278044</v>
+        <v>53.07588450546169</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_15</t>
+          <t>model_10_2_9</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.999937563787071</v>
+        <v>0.2841547080261584</v>
       </c>
       <c r="C17" t="n">
-        <v>0.6289749555397079</v>
+        <v>-0.7669979053490279</v>
       </c>
       <c r="D17" t="n">
-        <v>0.9997499028648069</v>
+        <v>-0.5943736838056117</v>
       </c>
       <c r="E17" t="n">
-        <v>0.9998198950693808</v>
+        <v>-31.36086922597636</v>
       </c>
       <c r="F17" t="n">
-        <v>0.999828640424672</v>
+        <v>-1.929148397792627</v>
       </c>
       <c r="G17" t="n">
-        <v>3.706483309859611e-05</v>
+        <v>0.4249566882221554</v>
       </c>
       <c r="H17" t="n">
-        <v>0.2202564938390141</v>
+        <v>1.048966286950237</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0001462148373721707</v>
+        <v>0.5823563501839477</v>
       </c>
       <c r="J17" t="n">
-        <v>6.158404122969027e-05</v>
+        <v>0.967077570072808</v>
       </c>
       <c r="K17" t="n">
-        <v>0.0001038994393009305</v>
+        <v>0.7747169601283779</v>
       </c>
       <c r="L17" t="n">
-        <v>0.001862565859407674</v>
+        <v>0.2567554364732467</v>
       </c>
       <c r="M17" t="n">
-        <v>0.006088089445679663</v>
+        <v>0.6518870210566824</v>
       </c>
       <c r="N17" t="n">
-        <v>1.000033299313562</v>
+        <v>-1.147535875921525</v>
       </c>
       <c r="O17" t="n">
-        <v>0.006347272017464781</v>
+        <v>0.6796392011352304</v>
       </c>
       <c r="P17" t="n">
-        <v>158.4056838656078</v>
+        <v>33.71153605063284</v>
       </c>
       <c r="Q17" t="n">
-        <v>242.5081157815137</v>
+        <v>53.21354924852405</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_16</t>
+          <t>model_10_2_7</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.9999315349880882</v>
+        <v>0.3016550307609261</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6288597441379106</v>
+        <v>-0.8847961782790832</v>
       </c>
       <c r="D18" t="n">
-        <v>0.9997190727872238</v>
+        <v>-0.4576974783100063</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9997935803314923</v>
+        <v>-28.88620210028903</v>
       </c>
       <c r="F18" t="n">
-        <v>0.9998063568259146</v>
+        <v>-1.694966616928822</v>
       </c>
       <c r="G18" t="n">
-        <v>4.064378860540695e-05</v>
+        <v>0.4145677406722181</v>
       </c>
       <c r="H18" t="n">
-        <v>0.2203248883039944</v>
+        <v>1.118896430381948</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0001642390933338176</v>
+        <v>0.5324343921148529</v>
       </c>
       <c r="J18" t="n">
-        <v>7.058195093435168e-05</v>
+        <v>0.893124208253722</v>
       </c>
       <c r="K18" t="n">
-        <v>0.0001174105221340847</v>
+        <v>0.7127793001842875</v>
       </c>
       <c r="L18" t="n">
-        <v>0.00192346730329522</v>
+        <v>0.2672418168419382</v>
       </c>
       <c r="M18" t="n">
-        <v>0.006375248121085715</v>
+        <v>0.643869350623415</v>
       </c>
       <c r="N18" t="n">
-        <v>1.00003651467302</v>
+        <v>-1.095034907717221</v>
       </c>
       <c r="O18" t="n">
-        <v>0.006646655632183274</v>
+        <v>0.6712802018727531</v>
       </c>
       <c r="P18" t="n">
-        <v>158.2213290709617</v>
+        <v>33.76103778064721</v>
       </c>
       <c r="Q18" t="n">
-        <v>242.3237609868675</v>
+        <v>53.26305097853842</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_17</t>
+          <t>model_10_2_6</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.9999246692973385</v>
+        <v>0.3008433607828547</v>
       </c>
       <c r="C19" t="n">
-        <v>0.6287512181838162</v>
+        <v>-1.21347089152998</v>
       </c>
       <c r="D19" t="n">
-        <v>0.9996857809198602</v>
+        <v>-0.4933107410538267</v>
       </c>
       <c r="E19" t="n">
-        <v>0.9997650348594811</v>
+        <v>-28.28380142154592</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9997822573617258</v>
+        <v>-1.68552518140267</v>
       </c>
       <c r="G19" t="n">
-        <v>4.47195592168135e-05</v>
+        <v>0.4150495830335188</v>
       </c>
       <c r="H19" t="n">
-        <v>0.220389313998422</v>
+        <v>1.314011938176014</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0001837025908610243</v>
+        <v>0.545442390127044</v>
       </c>
       <c r="J19" t="n">
-        <v>8.034262499929431e-05</v>
+        <v>0.8751219667026371</v>
       </c>
       <c r="K19" t="n">
-        <v>0.0001320226079301593</v>
+        <v>0.7102821784148404</v>
       </c>
       <c r="L19" t="n">
-        <v>0.001991452169273788</v>
+        <v>0.2796674628332683</v>
       </c>
       <c r="M19" t="n">
-        <v>0.006687268442107996</v>
+        <v>0.6442434190843697</v>
       </c>
       <c r="N19" t="n">
-        <v>1.000040176374753</v>
+        <v>-1.097469917651436</v>
       </c>
       <c r="O19" t="n">
-        <v>0.00697195930424258</v>
+        <v>0.671670195202519</v>
       </c>
       <c r="P19" t="n">
-        <v>158.0301991713547</v>
+        <v>33.75871457739814</v>
       </c>
       <c r="Q19" t="n">
-        <v>242.1326310872605</v>
+        <v>53.26072777528935</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_18</t>
+          <t>model_10_2_5</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.9999168659925483</v>
+        <v>0.2983574024328877</v>
       </c>
       <c r="C20" t="n">
-        <v>0.6286425053145974</v>
+        <v>-1.274302001888039</v>
       </c>
       <c r="D20" t="n">
-        <v>0.9996494498805066</v>
+        <v>-0.5059362617542824</v>
       </c>
       <c r="E20" t="n">
-        <v>0.9997336096505808</v>
+        <v>-28.31226607193137</v>
       </c>
       <c r="F20" t="n">
-        <v>0.9997558806678805</v>
+        <v>-1.695851278631731</v>
       </c>
       <c r="G20" t="n">
-        <v>4.935193802545849e-05</v>
+        <v>0.4165253552978683</v>
       </c>
       <c r="H20" t="n">
-        <v>0.2204538506537417</v>
+        <v>1.3501239130517</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0002049428861828412</v>
+        <v>0.5500539515376284</v>
       </c>
       <c r="J20" t="n">
-        <v>9.1087979687339e-05</v>
+        <v>0.875972609024248</v>
       </c>
       <c r="K20" t="n">
-        <v>0.0001480154329350901</v>
+        <v>0.7130132802809381</v>
       </c>
       <c r="L20" t="n">
-        <v>0.002070943270216533</v>
+        <v>0.2821156658779719</v>
       </c>
       <c r="M20" t="n">
-        <v>0.007025093453147687</v>
+        <v>0.6453877557700242</v>
       </c>
       <c r="N20" t="n">
-        <v>1.000044338137308</v>
+        <v>-1.104927792701337</v>
       </c>
       <c r="O20" t="n">
-        <v>0.00732416622539641</v>
+        <v>0.6728632486699853</v>
       </c>
       <c r="P20" t="n">
-        <v>157.8330670436466</v>
+        <v>33.75161588432493</v>
       </c>
       <c r="Q20" t="n">
-        <v>241.9354989595524</v>
+        <v>53.25362908221614</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_19</t>
+          <t>model_10_2_4</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.9999071768294662</v>
+        <v>0.2961077821119094</v>
       </c>
       <c r="C21" t="n">
-        <v>0.6285120224120599</v>
+        <v>-1.509387581580074</v>
       </c>
       <c r="D21" t="n">
-        <v>0.9996054888908831</v>
+        <v>-0.4941663949568207</v>
       </c>
       <c r="E21" t="n">
-        <v>0.9996965466197913</v>
+        <v>-28.61598099550729</v>
       </c>
       <c r="F21" t="n">
-        <v>0.9997242367671952</v>
+        <v>-1.704882475549504</v>
       </c>
       <c r="G21" t="n">
-        <v>5.510384378106935e-05</v>
+        <v>0.4178608270989389</v>
       </c>
       <c r="H21" t="n">
-        <v>0.2205313109412558</v>
+        <v>1.489680868325163</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0002306438960867077</v>
+        <v>0.5457549238128603</v>
       </c>
       <c r="J21" t="n">
-        <v>0.000103761098676297</v>
+        <v>0.8850488760501931</v>
       </c>
       <c r="K21" t="n">
-        <v>0.0001672018923564408</v>
+        <v>0.7154018999315267</v>
       </c>
       <c r="L21" t="n">
-        <v>0.002171095253770758</v>
+        <v>0.2811151147134043</v>
       </c>
       <c r="M21" t="n">
-        <v>0.007423196331841786</v>
+        <v>0.6464215552554996</v>
       </c>
       <c r="N21" t="n">
-        <v>1.000049505690951</v>
+        <v>-1.111676653664272</v>
       </c>
       <c r="O21" t="n">
-        <v>0.007739217167823083</v>
+        <v>0.6739410591398174</v>
       </c>
       <c r="P21" t="n">
-        <v>157.612582168293</v>
+        <v>33.7452137028429</v>
       </c>
       <c r="Q21" t="n">
-        <v>241.7150140841989</v>
+        <v>53.24722690073411</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_20</t>
+          <t>model_10_2_3</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.9998959042343297</v>
+        <v>0.2903361218192326</v>
       </c>
       <c r="C22" t="n">
-        <v>0.6283682125745449</v>
+        <v>-3.527570424552828</v>
       </c>
       <c r="D22" t="n">
-        <v>0.9995555635880414</v>
+        <v>-0.2364872736249253</v>
       </c>
       <c r="E22" t="n">
-        <v>0.9996538923394063</v>
+        <v>-24.47090993315279</v>
       </c>
       <c r="F22" t="n">
-        <v>0.9996881388217792</v>
+        <v>-1.292778193028434</v>
       </c>
       <c r="G22" t="n">
-        <v>6.179574320480719e-05</v>
+        <v>0.4212871339714144</v>
       </c>
       <c r="H22" t="n">
-        <v>0.2206166826730663</v>
+        <v>2.687761384873166</v>
       </c>
       <c r="I22" t="n">
-        <v>0.0002598318355251592</v>
+        <v>0.4516357884171553</v>
       </c>
       <c r="J22" t="n">
-        <v>0.000118346057304729</v>
+        <v>0.7611768866184887</v>
       </c>
       <c r="K22" t="n">
-        <v>0.0001890889464149442</v>
+        <v>0.606406337517822</v>
       </c>
       <c r="L22" t="n">
-        <v>0.002281296879963718</v>
+        <v>0.3261720214830092</v>
       </c>
       <c r="M22" t="n">
-        <v>0.007861026854349702</v>
+        <v>0.6490663555996523</v>
       </c>
       <c r="N22" t="n">
-        <v>1.000055517741691</v>
+        <v>-1.128991634542302</v>
       </c>
       <c r="O22" t="n">
-        <v>0.008195687042108289</v>
+        <v>0.6766984541101122</v>
       </c>
       <c r="P22" t="n">
-        <v>157.3833521521082</v>
+        <v>33.72888129867957</v>
       </c>
       <c r="Q22" t="n">
-        <v>241.485784068014</v>
+        <v>53.23089449657078</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_21</t>
+          <t>model_10_2_2</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.9998840131913197</v>
+        <v>0.289225631126796</v>
       </c>
       <c r="C23" t="n">
-        <v>0.6282264454431912</v>
+        <v>-4.091650536810659</v>
       </c>
       <c r="D23" t="n">
-        <v>0.9995035268117803</v>
+        <v>-0.2056400100316598</v>
       </c>
       <c r="E23" t="n">
-        <v>0.9996092608374532</v>
+        <v>-24.02526647217192</v>
       </c>
       <c r="F23" t="n">
-        <v>0.9996504663842313</v>
+        <v>-1.246301399625576</v>
       </c>
       <c r="G23" t="n">
-        <v>6.885478000186099e-05</v>
+        <v>0.4219463692171449</v>
       </c>
       <c r="H23" t="n">
-        <v>0.2207008417662591</v>
+        <v>3.022623706501495</v>
       </c>
       <c r="I23" t="n">
-        <v>0.0002902542103057267</v>
+        <v>0.4403686055592084</v>
       </c>
       <c r="J23" t="n">
-        <v>0.0001336070956726236</v>
+        <v>0.7478592036985792</v>
       </c>
       <c r="K23" t="n">
-        <v>0.0002119306529891751</v>
+        <v>0.5941139046288939</v>
       </c>
       <c r="L23" t="n">
-        <v>0.002389596795068657</v>
+        <v>0.3283269090673187</v>
       </c>
       <c r="M23" t="n">
-        <v>0.008297878042117816</v>
+        <v>0.6495739905639272</v>
       </c>
       <c r="N23" t="n">
-        <v>1.000061859631296</v>
+        <v>-1.132323106619612</v>
       </c>
       <c r="O23" t="n">
-        <v>0.008651135889346316</v>
+        <v>0.6772277001457654</v>
       </c>
       <c r="P23" t="n">
-        <v>157.1670218177669</v>
+        <v>33.72575412037109</v>
       </c>
       <c r="Q23" t="n">
-        <v>241.2694537336727</v>
+        <v>53.2277673182623</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_22</t>
+          <t>model_10_2_1</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.9998705162657691</v>
+        <v>0.2851785716141124</v>
       </c>
       <c r="C24" t="n">
-        <v>0.6280709718753552</v>
+        <v>-4.446654987007326</v>
       </c>
       <c r="D24" t="n">
-        <v>0.9994448749100038</v>
+        <v>-0.1773434451321201</v>
       </c>
       <c r="E24" t="n">
-        <v>0.9995594635990885</v>
+        <v>-23.19878607513798</v>
       </c>
       <c r="F24" t="n">
-        <v>0.9996081468994736</v>
+        <v>-1.180070522489379</v>
       </c>
       <c r="G24" t="n">
-        <v>7.686713804556204e-05</v>
+        <v>0.4243488785677419</v>
       </c>
       <c r="H24" t="n">
-        <v>0.2207931375922348</v>
+        <v>3.233369683531984</v>
       </c>
       <c r="I24" t="n">
-        <v>0.0003245440004435068</v>
+        <v>0.4300330835764909</v>
       </c>
       <c r="J24" t="n">
-        <v>0.0001506344761559049</v>
+        <v>0.7231605267719776</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0002375899762537687</v>
+        <v>0.5765968051742343</v>
       </c>
       <c r="L24" t="n">
-        <v>0.002508642240686956</v>
+        <v>0.3351128827800853</v>
       </c>
       <c r="M24" t="n">
-        <v>0.008767390606421161</v>
+        <v>0.6514206617599275</v>
       </c>
       <c r="N24" t="n">
-        <v>1.00006905799159</v>
+        <v>-1.144464285157663</v>
       </c>
       <c r="O24" t="n">
-        <v>0.009140636575537051</v>
+        <v>0.6791529879577158</v>
       </c>
       <c r="P24" t="n">
-        <v>156.9468642127869</v>
+        <v>33.71439867055173</v>
       </c>
       <c r="Q24" t="n">
-        <v>241.0492961286928</v>
+        <v>53.21641186844294</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>model_10_2_23</t>
+          <t>model_10_2_0</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.9998564009308277</v>
+        <v>0.1988080991765887</v>
       </c>
       <c r="C25" t="n">
-        <v>0.6279129610146548</v>
+        <v>-8.092972126574846</v>
       </c>
       <c r="D25" t="n">
-        <v>0.9993839367404692</v>
+        <v>0.4079537452445423</v>
       </c>
       <c r="E25" t="n">
-        <v>0.9995075589200286</v>
+        <v>-28.09970909941406</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9995641333701776</v>
+        <v>-1.052796998964697</v>
       </c>
       <c r="G25" t="n">
-        <v>8.524661061746527e-05</v>
+        <v>0.4756221220167947</v>
       </c>
       <c r="H25" t="n">
-        <v>0.2208869396648605</v>
+        <v>5.397981050278137</v>
       </c>
       <c r="I25" t="n">
-        <v>0.0003601704163214007</v>
+        <v>0.2162491137187512</v>
       </c>
       <c r="J25" t="n">
-        <v>0.0001683824627560286</v>
+        <v>0.869620521289872</v>
       </c>
       <c r="K25" t="n">
-        <v>0.0002642764395387146</v>
+        <v>0.5429348175043116</v>
       </c>
       <c r="L25" t="n">
-        <v>0.002627198167505669</v>
+        <v>0.2444372146048719</v>
       </c>
       <c r="M25" t="n">
-        <v>0.009232909109130516</v>
+        <v>0.6896536246673359</v>
       </c>
       <c r="N25" t="n">
-        <v>1.000076586170225</v>
+        <v>-1.403575702470234</v>
       </c>
       <c r="O25" t="n">
-        <v>0.009625973164662889</v>
+        <v>0.7190136072492366</v>
       </c>
       <c r="P25" t="n">
-        <v>156.7399244014879</v>
+        <v>33.48626320266946</v>
       </c>
       <c r="Q25" t="n">
-        <v>240.8423563173937</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>model_10_2_24</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>0.9998413779337549</v>
-      </c>
-      <c r="C26" t="n">
-        <v>0.6277469792053891</v>
-      </c>
-      <c r="D26" t="n">
-        <v>0.9993192050781585</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0.9994528944240605</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0.9995175088631498</v>
-      </c>
-      <c r="G26" t="n">
-        <v>9.416491063954567e-05</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0.2209854736368813</v>
-      </c>
-      <c r="I26" t="n">
-        <v>0.0003980146302116553</v>
-      </c>
-      <c r="J26" t="n">
-        <v>0.0001870741252326151</v>
-      </c>
-      <c r="K26" t="n">
-        <v>0.0002925460015319516</v>
-      </c>
-      <c r="L26" t="n">
-        <v>0.002747426957372333</v>
-      </c>
-      <c r="M26" t="n">
-        <v>0.009703860604911102</v>
-      </c>
-      <c r="N26" t="n">
-        <v>1.000084598435331</v>
-      </c>
-      <c r="O26" t="n">
-        <v>0.01011697404062285</v>
-      </c>
-      <c r="P26" t="n">
-        <v>156.5409258885908</v>
-      </c>
-      <c r="Q26" t="n">
-        <v>240.6433578044966</v>
+        <v>52.98827640056066</v>
       </c>
     </row>
   </sheetData>

</xml_diff>